<commit_message>
Se ha agregado el proyecto de correos aunque no se ha iniciado a trabajar y tambien se ha agregado una modificacion al proyecto de contabilidad y python para el tema de las facturas
</commit_message>
<xml_diff>
--- a/python/archivos_facturas.xlsx
+++ b/python/archivos_facturas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E341"/>
+  <dimension ref="A1:E362"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9640,6 +9640,573 @@
         </is>
       </c>
     </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>06.04.25</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Brindis</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>103,30</t>
+        </is>
+      </c>
+      <c r="D342" t="inlineStr">
+        <is>
+          <t>pdf</t>
+        </is>
+      </c>
+      <c r="E342" t="inlineStr">
+        <is>
+          <t>Facturas/2025/2T/ABRIL/06.04.25 Brindis 103,30.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>03.06.20</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Hotmart</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>555</t>
+        </is>
+      </c>
+      <c r="D343" t="inlineStr">
+        <is>
+          <t>pdf</t>
+        </is>
+      </c>
+      <c r="E343" t="inlineStr">
+        <is>
+          <t>Facturas/2025/2T/RESAGADAS/03.06.20 Hotmart 555.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>04.08.20</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Hotmart</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+      <c r="D344" t="inlineStr">
+        <is>
+          <t>pdf</t>
+        </is>
+      </c>
+      <c r="E344" t="inlineStr">
+        <is>
+          <t>Facturas/2025/2T/RESAGADAS/04.08.20 Hotmart 49.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>05.01.23</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Hotmart</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>90,21</t>
+        </is>
+      </c>
+      <c r="D345" t="inlineStr">
+        <is>
+          <t>pdf</t>
+        </is>
+      </c>
+      <c r="E345" t="inlineStr">
+        <is>
+          <t>Facturas/2025/2T/RESAGADAS/05.01.23 Hotmart 90,21.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>05.01.23</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Hotmart energia</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>90,21</t>
+        </is>
+      </c>
+      <c r="D346" t="inlineStr">
+        <is>
+          <t>pdf</t>
+        </is>
+      </c>
+      <c r="E346" t="inlineStr">
+        <is>
+          <t>Facturas/2025/2T/RESAGADAS/05.01.23 Hotmart energia 90,21.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>05.02.21</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Hotmart</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="D347" t="inlineStr">
+        <is>
+          <t>pdf</t>
+        </is>
+      </c>
+      <c r="E347" t="inlineStr">
+        <is>
+          <t>Facturas/2025/2T/RESAGADAS/05.02.21 Hotmart 97.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>05.12.22</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Hotmart</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>35,09</t>
+        </is>
+      </c>
+      <c r="D348" t="inlineStr">
+        <is>
+          <t>pdf</t>
+        </is>
+      </c>
+      <c r="E348" t="inlineStr">
+        <is>
+          <t>Facturas/2025/2T/RESAGADAS/05.12.22 Hotmart 35,09.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>06.04.21</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Hotmart</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>457,99</t>
+        </is>
+      </c>
+      <c r="D349" t="inlineStr">
+        <is>
+          <t>pdf</t>
+        </is>
+      </c>
+      <c r="E349" t="inlineStr">
+        <is>
+          <t>Facturas/2025/2T/RESAGADAS/06.04.21 Hotmart 457,99.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>07.10.24</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Atlas FZE</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>5000</t>
+        </is>
+      </c>
+      <c r="D350" t="inlineStr">
+        <is>
+          <t>pdf</t>
+        </is>
+      </c>
+      <c r="E350" t="inlineStr">
+        <is>
+          <t>Facturas/2025/2T/RESAGADAS/07.10.24 Atlas FZE 5000.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>07.12.22</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Hotmart</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>26,62</t>
+        </is>
+      </c>
+      <c r="D351" t="inlineStr">
+        <is>
+          <t>pdf</t>
+        </is>
+      </c>
+      <c r="E351" t="inlineStr">
+        <is>
+          <t>Facturas/2025/2T/RESAGADAS/07.12.22 Hotmart 26,62.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>07.12.22</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Hotmart</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>465,85</t>
+        </is>
+      </c>
+      <c r="D352" t="inlineStr">
+        <is>
+          <t>pdf</t>
+        </is>
+      </c>
+      <c r="E352" t="inlineStr">
+        <is>
+          <t>Facturas/2025/2T/RESAGADAS/07.12.22 Hotmart 465,85.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>17.02.21</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Hotmart</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>1,11</t>
+        </is>
+      </c>
+      <c r="D353" t="inlineStr">
+        <is>
+          <t>pdf</t>
+        </is>
+      </c>
+      <c r="E353" t="inlineStr">
+        <is>
+          <t>Facturas/2025/2T/RESAGADAS/17.02.21 Hotmart 1,11.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>19.01.24</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Hotmart</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>601,37</t>
+        </is>
+      </c>
+      <c r="D354" t="inlineStr">
+        <is>
+          <t>pdf</t>
+        </is>
+      </c>
+      <c r="E354" t="inlineStr">
+        <is>
+          <t>Facturas/2025/2T/RESAGADAS/19.01.24 Hotmart 601,37.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>19.08.22</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Hotmart</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>15,57</t>
+        </is>
+      </c>
+      <c r="D355" t="inlineStr">
+        <is>
+          <t>pdf</t>
+        </is>
+      </c>
+      <c r="E355" t="inlineStr">
+        <is>
+          <t>Facturas/2025/2T/RESAGADAS/19.08.22 Hotmart 15,57.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>19.10.20</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Hotmart</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>422,29</t>
+        </is>
+      </c>
+      <c r="D356" t="inlineStr">
+        <is>
+          <t>pdf</t>
+        </is>
+      </c>
+      <c r="E356" t="inlineStr">
+        <is>
+          <t>Facturas/2025/2T/RESAGADAS/19.10.20 Hotmart 422,29.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>19.10.20</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Hotmart</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="D357" t="inlineStr">
+        <is>
+          <t>pdf</t>
+        </is>
+      </c>
+      <c r="E357" t="inlineStr">
+        <is>
+          <t>Facturas/2025/2T/RESAGADAS/19.10.20 Hotmart 97.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>20.01.23</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Hotmart</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>111.32</t>
+        </is>
+      </c>
+      <c r="D358" t="inlineStr">
+        <is>
+          <t>pdf</t>
+        </is>
+      </c>
+      <c r="E358" t="inlineStr">
+        <is>
+          <t>Facturas/2025/2T/RESAGADAS/20.01.23 Hotmart 111.32.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>23.06.20</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Hotmart</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>3626,37</t>
+        </is>
+      </c>
+      <c r="D359" t="inlineStr">
+        <is>
+          <t>pdf</t>
+        </is>
+      </c>
+      <c r="E359" t="inlineStr">
+        <is>
+          <t>Facturas/2025/2T/RESAGADAS/23.06.20 Hotmart 3626,37.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>23.12.22</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Hotmart</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>1811.37</t>
+        </is>
+      </c>
+      <c r="D360" t="inlineStr">
+        <is>
+          <t>pdf</t>
+        </is>
+      </c>
+      <c r="E360" t="inlineStr">
+        <is>
+          <t>Facturas/2025/2T/RESAGADAS/23.12.22 Hotmart 1811.37.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>23.12.22</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Hotmart</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>81,07</t>
+        </is>
+      </c>
+      <c r="D361" t="inlineStr">
+        <is>
+          <t>pdf</t>
+        </is>
+      </c>
+      <c r="E361" t="inlineStr">
+        <is>
+          <t>Facturas/2025/2T/RESAGADAS/23.12.22 Hotmart 81,07.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>29.10.23</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Hotmart</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>671,55</t>
+        </is>
+      </c>
+      <c r="D362" t="inlineStr">
+        <is>
+          <t>pdf</t>
+        </is>
+      </c>
+      <c r="E362" t="inlineStr">
+        <is>
+          <t>Facturas/2025/2T/RESAGADAS/29.10.23 Hotmart 671,55.pdf</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>